<commit_message>
Can not read .env and can not login to gmail
</commit_message>
<xml_diff>
--- a/Jupyter/Web_Scraping/files/ArukeresoWebScraping.xlsx
+++ b/Jupyter/Web_Scraping/files/ArukeresoWebScraping.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -46,8 +48,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -432,6 +435,11 @@
           <t>Price</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -439,10 +447,11 @@
           <t>LG UltraGear 24GN60R-B</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>54 590</t>
-        </is>
+      <c r="B2" t="n">
+        <v>54590</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>45326</v>
       </c>
     </row>
   </sheetData>

</xml_diff>